<commit_message>
Industry PAMs tweaks and REF fix
Clinker substitution in REF industry was set to high pam. reset that and fixed bug in ref substitution spreadsheet. 

made fixes and edits to industry PAM sheet for scenario runs.
</commit_message>
<xml_diff>
--- a/SATIM/DataSpreadsheets/TCH_IND/TCH_IND_ALM.xlsx
+++ b/SATIM/DataSpreadsheets/TCH_IND/TCH_IND_ALM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Models\SATIMGE\SATIM\DataSpreadsheets\TCH_IND\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B83B03BC-7934-40F2-A2F3-AD1010ACDB47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95DECCE9-626E-479B-86C4-2306EA45A171}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="796" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -45,6 +45,7 @@
   </sheets>
   <externalReferences>
     <externalReference r:id="rId30"/>
+    <externalReference r:id="rId31"/>
   </externalReferences>
   <definedNames>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" localSheetId="8" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
@@ -257,6 +258,28 @@
     </comment>
   </commentList>
 </comments>
+</file>
+
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -10607,6 +10630,354 @@
 </externalLink>
 </file>
 
+<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Index"/>
+      <sheetName val="ChangeLog"/>
+      <sheetName val="NameConv"/>
+      <sheetName val="Industry desription"/>
+      <sheetName val="SIC codes"/>
+      <sheetName val="REGIONS"/>
+      <sheetName val="Detailed GDP STATSSA"/>
+      <sheetName val="GDP STATSSA"/>
+      <sheetName val="Output compiled"/>
+      <sheetName val="IND GDP statssa 2"/>
+      <sheetName val="Ind output Mark"/>
+      <sheetName val="Ind mining output STATSSA"/>
+      <sheetName val="Ind Man output STATSSA"/>
+      <sheetName val="supply and use tables"/>
+      <sheetName val="DOE 2006 native units"/>
+      <sheetName val="2006-2009"/>
+      <sheetName val="Industry VA"/>
+      <sheetName val="Sources"/>
+      <sheetName val="1992-2006 industry"/>
+      <sheetName val="DoE2013 Industry EB"/>
+      <sheetName val="digest "/>
+      <sheetName val="DMR1"/>
+      <sheetName val="mining general info"/>
+      <sheetName val="I&amp;S - prod"/>
+      <sheetName val="I&amp;S - prod 2"/>
+      <sheetName val="I&amp;S - prod 3"/>
+      <sheetName val="End uses"/>
+      <sheetName val="EIA end use"/>
+      <sheetName val="Aluminium"/>
+      <sheetName val="Eskom sales data"/>
+      <sheetName val="Eskom Annual YB"/>
+      <sheetName val="eskom yb sector sales"/>
+      <sheetName val="NERSA Elec"/>
+      <sheetName val="REPORT TABLES"/>
+      <sheetName val="Tech Efficiencies"/>
+      <sheetName val="Coal prices"/>
+      <sheetName val="Electricity prices"/>
+      <sheetName val="ELEC CALCS ADRIAN IGNORE"/>
+      <sheetName val="FA-Items"/>
+      <sheetName val="FA-TSData"/>
+      <sheetName val="FA-TIDData"/>
+      <sheetName val="FerroAlloys"/>
+      <sheetName val="Aluminium - Items"/>
+      <sheetName val="Aluminium - TIDData"/>
+      <sheetName val="Aluminium - TSData"/>
+      <sheetName val="Aluminium Data"/>
+      <sheetName val="NMM-Items"/>
+      <sheetName val="NMM-TSData"/>
+      <sheetName val="NMM-TIDData"/>
+      <sheetName val="NMM data"/>
+      <sheetName val="Coking coal"/>
+      <sheetName val="COGEN"/>
+      <sheetName val="Payback from EIA"/>
+      <sheetName val="SasolGasSales"/>
+      <sheetName val="2012 SATIM EB"/>
+      <sheetName val="2017 SATIM EB"/>
+      <sheetName val="IND old - 2006BY"/>
+      <sheetName val="IND"/>
+      <sheetName val="IND2017"/>
+      <sheetName val="PAMS central control panel"/>
+      <sheetName val="ITEMS_Tech"/>
+      <sheetName val="ITEMS_Comm"/>
+      <sheetName val="TS DTech"/>
+      <sheetName val="TS DMARK"/>
+      <sheetName val="TID DTech"/>
+      <sheetName val="TS BYDem"/>
+      <sheetName val="TS COMFRN"/>
+      <sheetName val="TS COMFR"/>
+      <sheetName val="TS COMFRN_10"/>
+      <sheetName val="TS COMFR_10"/>
+      <sheetName val="TS ETech"/>
+      <sheetName val="TID ETech"/>
+      <sheetName val="TS GTech"/>
+      <sheetName val="TID GTech"/>
+      <sheetName val="TS FTech"/>
+      <sheetName val="TID FTech"/>
+      <sheetName val="TS Emiss"/>
+      <sheetName val="TID Emiss"/>
+      <sheetName val="AFA"/>
+      <sheetName val="Sc1 Standards"/>
+      <sheetName val="Sc2 Audits"/>
+      <sheetName val="Sc3 En Man"/>
+      <sheetName val="Sc4 Accreditation"/>
+      <sheetName val="Sc5 Education"/>
+      <sheetName val="Sc6 NEEA"/>
+      <sheetName val="Sc7 Finance"/>
+    </sheetNames>
+    <definedNames>
+      <definedName name="pamsindex" refersTo="='PAMS central control panel'!$C$2"/>
+    </definedNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
+      <sheetData sheetId="7">
+        <row r="2">
+          <cell r="C2" t="str">
+            <v>Agriculture, forestry and fishing</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="8"/>
+      <sheetData sheetId="9">
+        <row r="2">
+          <cell r="C2" t="str">
+            <v>1994</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="10"/>
+      <sheetData sheetId="11">
+        <row r="2">
+          <cell r="C2" t="str">
+            <v>FMP20000</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="12"/>
+      <sheetData sheetId="13"/>
+      <sheetData sheetId="14">
+        <row r="2">
+          <cell r="C2">
+            <v>813472</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="15">
+        <row r="2">
+          <cell r="C2">
+            <v>1</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="16"/>
+      <sheetData sheetId="17"/>
+      <sheetData sheetId="18">
+        <row r="2">
+          <cell r="C2">
+            <v>1992</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="19"/>
+      <sheetData sheetId="20"/>
+      <sheetData sheetId="21"/>
+      <sheetData sheetId="22"/>
+      <sheetData sheetId="23"/>
+      <sheetData sheetId="24"/>
+      <sheetData sheetId="25"/>
+      <sheetData sheetId="26"/>
+      <sheetData sheetId="27"/>
+      <sheetData sheetId="28"/>
+      <sheetData sheetId="29"/>
+      <sheetData sheetId="30">
+        <row r="2">
+          <cell r="C2">
+            <v>1988</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="31"/>
+      <sheetData sheetId="32">
+        <row r="2">
+          <cell r="C2">
+            <v>1996</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="33"/>
+      <sheetData sheetId="34"/>
+      <sheetData sheetId="35"/>
+      <sheetData sheetId="36"/>
+      <sheetData sheetId="37"/>
+      <sheetData sheetId="38">
+        <row r="2">
+          <cell r="C2" t="str">
+            <v>IFAEAF_CG-I</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="39">
+        <row r="2">
+          <cell r="C2" t="str">
+            <v>-</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="40">
+        <row r="2">
+          <cell r="C2" t="str">
+            <v>-</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="41"/>
+      <sheetData sheetId="42">
+        <row r="2">
+          <cell r="C2" t="str">
+            <v>IALPOT_CG-I</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="43">
+        <row r="2">
+          <cell r="C2" t="str">
+            <v>-</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="44">
+        <row r="2">
+          <cell r="C2" t="str">
+            <v>-</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="45"/>
+      <sheetData sheetId="46">
+        <row r="2">
+          <cell r="C2" t="str">
+            <v>UC-INM-KLD</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="47"/>
+      <sheetData sheetId="48">
+        <row r="2">
+          <cell r="C2" t="str">
+            <v>-</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="49"/>
+      <sheetData sheetId="50">
+        <row r="2">
+          <cell r="C2">
+            <v>2001</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="51"/>
+      <sheetData sheetId="52">
+        <row r="2">
+          <cell r="C2" t="str">
+            <v>High Temperature Heat</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="53">
+        <row r="2">
+          <cell r="C2">
+            <v>2006</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="54"/>
+      <sheetData sheetId="55"/>
+      <sheetData sheetId="56"/>
+      <sheetData sheetId="57"/>
+      <sheetData sheetId="58"/>
+      <sheetData sheetId="59">
+        <row r="2">
+          <cell r="C2" t="b">
+            <v>0</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="60"/>
+      <sheetData sheetId="61"/>
+      <sheetData sheetId="62"/>
+      <sheetData sheetId="63"/>
+      <sheetData sheetId="64"/>
+      <sheetData sheetId="65"/>
+      <sheetData sheetId="66"/>
+      <sheetData sheetId="67"/>
+      <sheetData sheetId="68"/>
+      <sheetData sheetId="69"/>
+      <sheetData sheetId="70"/>
+      <sheetData sheetId="71"/>
+      <sheetData sheetId="72"/>
+      <sheetData sheetId="73"/>
+      <sheetData sheetId="74"/>
+      <sheetData sheetId="75"/>
+      <sheetData sheetId="76"/>
+      <sheetData sheetId="77"/>
+      <sheetData sheetId="78"/>
+      <sheetData sheetId="79">
+        <row r="2">
+          <cell r="C2">
+            <v>2012</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="80">
+        <row r="2">
+          <cell r="C2">
+            <v>2012</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="81">
+        <row r="2">
+          <cell r="C2">
+            <v>2012</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="82">
+        <row r="2">
+          <cell r="C2">
+            <v>2012</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="83">
+        <row r="2">
+          <cell r="C2">
+            <v>2012</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="84">
+        <row r="2">
+          <cell r="C2">
+            <v>2012</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="85">
+        <row r="2">
+          <cell r="C2">
+            <v>2012</v>
+          </cell>
+        </row>
+      </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -19613,7 +19984,7 @@
   <dimension ref="B3:N27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G28" sqref="G28:G29"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -19694,7 +20065,8 @@
       <c r="I9" s="94" t="s">
         <v>370</v>
       </c>
-      <c r="J9" t="b">
+      <c r="J9" t="b" cm="1">
+        <f t="array" ref="J9">[2]!pamsindex</f>
         <v>0</v>
       </c>
     </row>
@@ -19807,10 +20179,7 @@
       <c r="E27" s="125"/>
     </row>
   </sheetData>
-  <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J9" xr:uid="{649E72FB-A0B3-4F01-B5FA-D6C888ACD94C}">
-      <formula1>"TRUE,FALSE"</formula1>
-    </dataValidation>
+  <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J10" xr:uid="{158ECA61-51EF-4EA1-B317-22BEED597959}">
       <formula1>$I$12:$I$13</formula1>
     </dataValidation>

</xml_diff>